<commit_message>
More changes to get Jenkins green
</commit_message>
<xml_diff>
--- a/Prototypes/Grapevine/Observations/PhenoDataObservation.xlsx
+++ b/Prototypes/Grapevine/Observations/PhenoDataObservation.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Grapevine\Observations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Prototypes\Grapevine\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="360" windowWidth="27552" windowHeight="12300"/>
+    <workbookView xWindow="600" yWindow="360" windowWidth="27555" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$C$1:$H$61</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -67,25 +67,25 @@
     <t>Grapevine.Phenology.CurrentStageName</t>
   </si>
   <si>
-    <t>Grapevine.Phenology.BudBurstDOY.Value</t>
-  </si>
-  <si>
-    <t>Grapevine.Phenology.FloweringDOY.Value</t>
-  </si>
-  <si>
-    <t>Grapevine.Phenology.VeraisonDOY.Value</t>
-  </si>
-  <si>
     <t>SimulationName</t>
   </si>
   <si>
     <t>Clock.Today.Year</t>
   </si>
+  <si>
+    <t>Grapevine.Phenology.BudBurstDOY.Value()</t>
+  </si>
+  <si>
+    <t>Grapevine.Phenology.FloweringDOY.Value()</t>
+  </si>
+  <si>
+    <t>Grapevine.Phenology.VeraisonDOY.Value()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -212,6 +212,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -247,6 +264,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,24 +459,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
@@ -451,22 +485,22 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>VLOOKUP(E2,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -488,7 +522,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>VLOOKUP(E3,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -510,7 +544,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>VLOOKUP(E4,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -532,7 +566,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>VLOOKUP(E5,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -554,7 +588,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>VLOOKUP(E6,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -576,7 +610,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>VLOOKUP(E7,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -598,7 +632,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>VLOOKUP(E8,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -620,7 +654,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>VLOOKUP(E9,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -642,7 +676,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>VLOOKUP(E10,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -664,7 +698,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>VLOOKUP(E11,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -686,7 +720,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>VLOOKUP(E12,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -713,7 +747,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>VLOOKUP(E13,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -740,7 +774,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>VLOOKUP(E14,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -767,7 +801,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>VLOOKUP(E15,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -794,7 +828,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>VLOOKUP(E16,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -821,7 +855,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>VLOOKUP(E17,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -848,7 +882,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>VLOOKUP(E18,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -875,7 +909,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>VLOOKUP(E19,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -902,7 +936,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>VLOOKUP(E20,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -929,7 +963,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>VLOOKUP(E21,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -956,7 +990,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>VLOOKUP(E22,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -983,7 +1017,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>VLOOKUP(E23,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -1010,7 +1044,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>VLOOKUP(E24,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -1037,7 +1071,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>VLOOKUP(E25,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -1064,7 +1098,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>VLOOKUP(E26,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -1091,7 +1125,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>VLOOKUP(E27,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -1118,7 +1152,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>VLOOKUP(E28,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -1145,7 +1179,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>VLOOKUP(E29,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -1172,7 +1206,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>VLOOKUP(E30,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -1199,7 +1233,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>VLOOKUP(E31,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -1226,7 +1260,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>VLOOKUP(E32,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -1253,7 +1287,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>VLOOKUP(E33,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -1280,7 +1314,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>VLOOKUP(E34,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -1307,7 +1341,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>VLOOKUP(E35,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -1334,7 +1368,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>VLOOKUP(E36,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -1361,7 +1395,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>VLOOKUP(E37,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -1388,7 +1422,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>VLOOKUP(E38,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -1415,7 +1449,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>VLOOKUP(E39,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -1442,7 +1476,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>VLOOKUP(E40,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -1469,7 +1503,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>VLOOKUP(E41,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -1496,7 +1530,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>VLOOKUP(E42,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -1523,7 +1557,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>VLOOKUP(E43,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -1550,7 +1584,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>VLOOKUP(E44,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -1577,7 +1611,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>VLOOKUP(E45,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -1604,7 +1638,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>VLOOKUP(E46,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -1631,7 +1665,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>VLOOKUP(E47,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -1658,7 +1692,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>VLOOKUP(E48,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -1685,7 +1719,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>VLOOKUP(E49,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -1712,7 +1746,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>VLOOKUP(E50,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -1739,7 +1773,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>VLOOKUP(E51,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -1766,7 +1800,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>VLOOKUP(E52,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -1793,7 +1827,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>VLOOKUP(E53,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -1820,7 +1854,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>VLOOKUP(E54,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -1847,7 +1881,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>VLOOKUP(E55,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -1874,7 +1908,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>VLOOKUP(E56,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -1901,7 +1935,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>VLOOKUP(E57,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1001.met</v>
@@ -1925,7 +1959,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>VLOOKUP(E58,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1002.met</v>
@@ -1949,7 +1983,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>VLOOKUP(E59,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1003.met</v>
@@ -1973,7 +2007,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>VLOOKUP(E60,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1004.met</v>
@@ -1997,7 +2031,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>VLOOKUP(E61,'New input phenodata'!$A$1:$B$5, 2,FALSE )</f>
         <v>PhenoTestClimateSite1005.met</v>
@@ -2035,12 +2069,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.21875" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2048,7 +2082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2056,7 +2090,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2064,7 +2098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2072,7 +2106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>

</xml_diff>